<commit_message>
Upgrade the detial design document
</commit_message>
<xml_diff>
--- a/Documents/Design/VoteInterfaceDocument.xlsx
+++ b/Documents/Design/VoteInterfaceDocument.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="624" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000" tabRatio="624" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,11 @@
     <sheet name="InitialVote" sheetId="5" r:id="rId5"/>
     <sheet name="JoinVote" sheetId="6" r:id="rId6"/>
     <sheet name="SearchVote" sheetId="7" r:id="rId7"/>
-    <sheet name="IndexVoteHistory" sheetId="9" r:id="rId8"/>
+    <sheet name="IndexVoteHistoryList" sheetId="9" r:id="rId8"/>
     <sheet name="ViewProcessingVote" sheetId="8" r:id="rId9"/>
     <sheet name="SetPassword" sheetId="10" r:id="rId10"/>
-    <sheet name="CancelVote" sheetId="11" r:id="rId11"/>
-    <sheet name="ViewDuplicateVote" sheetId="12" r:id="rId12"/>
+    <sheet name="CancelUserSelection" sheetId="11" r:id="rId11"/>
+    <sheet name="ViewDuplicateSelection" sheetId="12" r:id="rId12"/>
     <sheet name="CodeCheck" sheetId="13" r:id="rId13"/>
     <sheet name="ViewHistoryVote" sheetId="14" r:id="rId14"/>
     <sheet name="ViewVoteParticipator" sheetId="15" r:id="rId15"/>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1673,7 +1673,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2091,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2206,7 +2206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -3182,7 +3182,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Upload sample UI,upgrade interface document
</commit_message>
<xml_diff>
--- a/Documents/Design/VoteInterfaceDocument.xlsx
+++ b/Documents/Design/VoteInterfaceDocument.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="624" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="624" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="153">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -606,6 +606,42 @@
   </si>
   <si>
     <t>Bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>firstName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:signIn 1:signUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resendType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -835,7 +871,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -925,8 +961,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -965,6 +1007,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1019,7 +1064,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="95">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -1065,6 +1110,9 @@
     <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1109,6 +1157,9 @@
     <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1449,40 +1500,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="39" customHeight="1" thickBot="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="5" t="s">
@@ -1497,10 +1548,10 @@
       <c r="D5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" ht="62" thickTop="1" thickBot="1">
       <c r="A6" s="6" t="s">
@@ -1515,10 +1566,10 @@
       <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="6" t="s">
@@ -1531,18 +1582,18 @@
         <v>11</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" ht="16" thickTop="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1581,12 +1632,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1628,12 +1679,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1683,12 +1734,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1730,12 +1781,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1797,12 +1848,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1832,12 +1883,12 @@
     </row>
     <row r="5" spans="1:5" ht="16" thickBot="1"/>
     <row r="6" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:5" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -1854,13 +1905,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1868,17 +1919,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" thickBot="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="7" t="s">
         <v>127</v>
       </c>
@@ -1922,12 +1973,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1983,12 +2034,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -2039,12 +2090,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="10" t="s">
@@ -2086,12 +2137,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
@@ -2108,13 +2159,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" thickBot="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -2122,25 +2173,25 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="9" t="s">
         <v>119</v>
       </c>
@@ -2158,13 +2209,13 @@
       <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>116</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -2172,17 +2223,17 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="9" t="s">
         <v>120</v>
       </c>
@@ -2228,12 +2279,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2263,12 +2314,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="2" t="s">
@@ -2285,13 +2336,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="31" thickBot="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2299,9 +2350,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="2" t="s">
         <v>125</v>
       </c>
@@ -2344,12 +2395,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -2391,12 +2442,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
@@ -2430,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2447,66 +2498,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" ht="16" thickBot="1">
+      <c r="A4" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="15"/>
+    </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1">
+      <c r="A6" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1"/>
+    <row r="9" spans="1:4" ht="16" thickBot="1">
+      <c r="A9" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-    </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="14" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1">
+      <c r="A10" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2538,12 +2627,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="14" t="s">
@@ -2573,12 +2662,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="14" t="s">
@@ -2632,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2646,12 +2735,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2705,12 +2794,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -2759,7 +2848,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2772,12 +2861,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2807,12 +2896,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="13" t="s">
@@ -2860,7 +2949,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2873,12 +2962,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2920,12 +3009,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -2974,12 +3063,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3107,12 +3196,12 @@
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1"/>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="7" t="s">
@@ -3174,12 +3263,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3221,12 +3310,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -3276,12 +3365,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3349,12 +3438,12 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="7" t="s">
@@ -3371,13 +3460,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="76" thickBot="1">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -3385,25 +3474,25 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="7" t="s">
         <v>84</v>
       </c>
@@ -3445,12 +3534,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3480,12 +3569,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="10" t="s">
@@ -3502,13 +3591,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>86</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -3516,65 +3605,65 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" thickBot="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="10" t="s">
         <v>129</v>
       </c>
@@ -3615,12 +3704,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3664,12 +3753,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -3734,13 +3823,13 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="27" t="s">
         <v>86</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -3748,17 +3837,17 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="7" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Update the interface document, complete vote search client code
</commit_message>
<xml_diff>
--- a/Documents/Design/VoteInterfaceDocument.xlsx
+++ b/Documents/Design/VoteInterfaceDocument.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="624" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="624" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="159">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -654,6 +654,18 @@
   </si>
   <si>
     <t>hasPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchtype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -883,7 +895,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -981,8 +993,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1027,6 +1041,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1081,7 +1098,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="99">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -1131,6 +1148,7 @@
     <cellStyle name="访问过的超链接" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1179,6 +1197,7 @@
     <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1519,40 +1538,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="39" customHeight="1" thickBot="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="5" t="s">
@@ -1567,10 +1586,10 @@
       <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" ht="62" thickTop="1" thickBot="1">
       <c r="A6" s="6" t="s">
@@ -1585,10 +1604,10 @@
       <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="6" t="s">
@@ -1601,18 +1620,18 @@
         <v>11</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:6" ht="16" thickTop="1">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1651,12 +1670,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1698,12 +1717,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1753,12 +1772,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1800,12 +1819,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1867,12 +1886,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1902,12 +1921,12 @@
     </row>
     <row r="5" spans="1:5" ht="16" thickBot="1"/>
     <row r="6" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:5" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -1924,13 +1943,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1938,17 +1957,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" thickBot="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="7" t="s">
         <v>126</v>
       </c>
@@ -1977,7 +1996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -1992,12 +2011,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2053,12 +2072,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="15" t="s">
@@ -2135,12 +2154,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="10" t="s">
@@ -2182,12 +2201,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
@@ -2204,13 +2223,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" thickBot="1">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -2218,25 +2237,25 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="9" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="9" t="s">
         <v>118</v>
       </c>
@@ -2254,13 +2273,13 @@
       <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="31" t="s">
         <v>115</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -2268,17 +2287,17 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="9" t="s">
         <v>119</v>
       </c>
@@ -2324,12 +2343,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2359,12 +2378,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="2" t="s">
@@ -2381,13 +2400,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="31" thickBot="1">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="30" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2395,9 +2414,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="2" t="s">
         <v>124</v>
       </c>
@@ -2440,12 +2459,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -2487,12 +2506,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
@@ -2543,12 +2562,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="16" t="s">
@@ -2616,12 +2635,12 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="14" t="s">
@@ -2672,12 +2691,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="14" t="s">
@@ -2707,12 +2726,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="14" t="s">
@@ -2780,12 +2799,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2839,12 +2858,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -2894,12 +2913,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2929,12 +2948,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="13" t="s">
@@ -2983,12 +3002,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3030,12 +3049,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="15" t="s">
@@ -3096,12 +3115,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3229,12 +3248,12 @@
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1"/>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="7" t="s">
@@ -3296,12 +3315,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3343,12 +3362,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -3382,10 +3401,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3398,12 +3417,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3471,63 +3490,77 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="76" thickBot="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="7" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="7" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="17" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" thickBot="1">
+      <c r="A15" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3567,12 +3600,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3602,12 +3635,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="10" t="s">
@@ -3624,13 +3657,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="30" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -3638,65 +3671,65 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" thickBot="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="10" t="s">
         <v>128</v>
       </c>
@@ -3737,12 +3770,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3786,12 +3819,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -3856,13 +3889,13 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>85</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -3870,17 +3903,17 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="7" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Add dev certificate, upgrade interface doc
</commit_message>
<xml_diff>
--- a/Documents/Design/VoteInterfaceDocument.xlsx
+++ b/Documents/Design/VoteInterfaceDocument.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="158">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,7 +281,379 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>longtitude</t>
+    <t>voteid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>votelist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initiator:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>color:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:location 1:id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>starttime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All time format is yy:mm:dd:hh:mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxvaliduser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteid:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If the user has already vote, they don't have to input the password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selection's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectionlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contentid:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>historylist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>history's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>color:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>currentvalidvote:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxvaliduser:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createtime:datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endtime:datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vote's subkey, if user has already joined this vote, don't return that vote record.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>votefnished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicatelist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicate's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteoptionid:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checktype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:signup 1:signin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pollnumber:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userselection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userselection's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dictionary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteoptionid:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finaloptionid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>participatorlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>participator's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slectionlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emaillist:array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initiatorid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tokenid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>firstName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:signIn 1:signUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resendType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return when use Email signin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hasPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchtype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -289,383 +661,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>color</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(45)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>votelist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>initiator:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>color:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:location 1:id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>starttime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All time format is yy:mm:dd:hh:mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxvaliduser</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteid:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If the user has already vote, they don't have to input the password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>selection's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectionlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>content:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>contentid:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>historylist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>history's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>title:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>color:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>currentvalidvote:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxvaliduser:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>createtime:datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>endtime:datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vote's subkey, if user has already joined this vote, don't return that vote record.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>votefnished</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicatelist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicate's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteoptionid:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(255)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>checktype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:signup 1:signin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pollnumber:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userselection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userselection's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dictionary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteoptionid:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>finaloptionid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>participatorlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>participator's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>slectionlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>emaillist:array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Request Content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>initiatorid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tokenid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lastName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>firstName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lastName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:signIn 1:signUp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>resendType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>return when use Email signin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hasPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchtype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>longitude</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1625,7 +1621,7 @@
     </row>
     <row r="8" spans="1:6" ht="16" thickTop="1">
       <c r="A8" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -1696,7 +1692,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -1705,10 +1701,10 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>35</v>
@@ -1795,10 +1791,10 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -1810,7 +1806,7 @@
         <v>37</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>35</v>
@@ -1842,10 +1838,10 @@
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
       <c r="A9" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>34</v>
@@ -1912,7 +1908,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -1944,7 +1940,7 @@
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
       <c r="A8" s="29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>56</v>
@@ -1953,7 +1949,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" thickBot="1">
@@ -1961,7 +1957,7 @@
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" thickBot="1">
@@ -1969,7 +1965,7 @@
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -2037,7 +2033,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -2046,7 +2042,7 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>24</v>
@@ -2058,7 +2054,7 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>53</v>
@@ -2067,7 +2063,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
@@ -2095,28 +2091,28 @@
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
       <c r="A9" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="31" thickBot="1">
       <c r="A10" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2180,7 +2176,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>12</v>
@@ -2189,13 +2185,13 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D4" s="9"/>
     </row>
@@ -2224,16 +2220,16 @@
     </row>
     <row r="8" spans="1:4" ht="31" thickBot="1">
       <c r="A8" s="31" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
@@ -2241,7 +2237,7 @@
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
@@ -2249,7 +2245,7 @@
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
@@ -2257,15 +2253,15 @@
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
       <c r="D11" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>18</v>
@@ -2274,16 +2270,16 @@
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
       <c r="A13" s="31" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
@@ -2291,7 +2287,7 @@
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
@@ -2299,7 +2295,7 @@
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
       <c r="D15" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2397,7 @@
     </row>
     <row r="7" spans="1:4" ht="31" thickBot="1">
       <c r="A7" s="30" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>56</v>
@@ -2410,7 +2406,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
@@ -2418,7 +2414,7 @@
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2482,7 +2478,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>42</v>
@@ -2494,13 +2490,13 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -2524,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2588,7 +2584,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>12</v>
@@ -2597,40 +2593,40 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
@@ -2714,7 +2710,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>42</v>
@@ -2800,7 +2796,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
       <c r="A1" s="26" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2822,7 +2818,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -2846,7 +2842,7 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -3072,13 +3068,13 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -3236,7 +3232,7 @@
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
       <c r="A11" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>53</v>
@@ -3404,7 +3400,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3449,15 +3445,15 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>36</v>
@@ -3466,10 +3462,10 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="7" t="s">
-        <v>63</v>
+        <v>156</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -3478,7 +3474,7 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>53</v>
@@ -3513,7 +3509,7 @@
     </row>
     <row r="11" spans="1:4" ht="76" thickBot="1">
       <c r="A11" s="30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>56</v>
@@ -3522,7 +3518,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
@@ -3530,7 +3526,7 @@
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
@@ -3538,7 +3534,7 @@
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
@@ -3546,21 +3542,21 @@
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
       <c r="D14" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
       <c r="A15" s="17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3626,7 +3622,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -3658,16 +3654,16 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
@@ -3675,7 +3671,7 @@
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
@@ -3683,7 +3679,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
@@ -3691,7 +3687,7 @@
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
@@ -3699,7 +3695,7 @@
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
@@ -3707,7 +3703,7 @@
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
@@ -3715,7 +3711,7 @@
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
       <c r="D14" s="10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
@@ -3723,7 +3719,7 @@
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" thickBot="1">
@@ -3731,7 +3727,7 @@
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
       <c r="D16" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3793,10 +3789,10 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -3805,16 +3801,16 @@
     </row>
     <row r="4" spans="1:4" ht="76" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
@@ -3845,7 +3841,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>34</v>
@@ -3854,13 +3850,13 @@
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -3869,7 +3865,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>18</v>
@@ -3878,7 +3874,7 @@
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
       <c r="A12" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>53</v>
@@ -3890,16 +3886,16 @@
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
       <c r="A13" s="29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
@@ -3907,7 +3903,7 @@
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
@@ -3915,7 +3911,7 @@
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix property spelling error, update interface doc
</commit_message>
<xml_diff>
--- a/Documents/Design/VoteInterfaceDocument.xlsx
+++ b/Documents/Design/VoteInterfaceDocument.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25560" windowHeight="14080" tabRatio="624" firstSheet="10" activeTab="13"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25560" windowHeight="14080" tabRatio="624" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="164">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -675,6 +675,18 @@
   </si>
   <si>
     <t>slectionlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servercurrentime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1009,7 +1021,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1054,6 +1066,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1564,40 +1579,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" ht="39" customHeight="1" thickBot="1">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="5" t="s">
@@ -1612,10 +1627,10 @@
       <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:6" ht="62" thickTop="1" thickBot="1">
       <c r="A6" s="6" t="s">
@@ -1630,10 +1645,10 @@
       <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="6" t="s">
@@ -1646,18 +1661,18 @@
         <v>11</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" ht="16" thickTop="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1696,12 +1711,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1743,12 +1758,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1798,12 +1813,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1845,12 +1860,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1900,12 +1915,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1935,12 +1950,12 @@
     </row>
     <row r="5" spans="1:5" ht="16" thickBot="1"/>
     <row r="6" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:5" ht="16" thickBot="1">
       <c r="A7" s="18" t="s">
@@ -1957,13 +1972,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -1971,17 +1986,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="18" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" thickBot="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="18" t="s">
         <v>110</v>
       </c>
@@ -2025,12 +2040,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2086,12 +2101,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="15" t="s">
@@ -2153,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2168,12 +2183,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="10" t="s">
@@ -2215,12 +2230,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
@@ -2237,13 +2252,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" thickBot="1">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -2251,37 +2266,37 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="9" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>102</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -2289,17 +2304,17 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="9" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="9" t="s">
         <v>106</v>
       </c>
@@ -2345,12 +2360,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2380,12 +2395,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="2" t="s">
@@ -2402,13 +2417,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="31" thickBot="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2416,9 +2431,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="2" t="s">
         <v>109</v>
       </c>
@@ -2461,12 +2476,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -2508,12 +2523,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
@@ -2564,12 +2579,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="16" t="s">
@@ -2637,12 +2652,12 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="14" t="s">
@@ -2693,12 +2708,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="14" t="s">
@@ -2728,12 +2743,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="14" t="s">
@@ -2801,12 +2816,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2860,12 +2875,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -2916,12 +2931,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="19" t="s">
@@ -2951,12 +2966,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="19" t="s">
@@ -3005,12 +3020,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3040,12 +3055,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="13" t="s">
@@ -3094,12 +3109,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3141,12 +3156,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="15" t="s">
@@ -3207,12 +3222,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3340,12 +3355,12 @@
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1"/>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="7" t="s">
@@ -3407,12 +3422,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3454,12 +3469,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -3509,12 +3524,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3582,12 +3597,12 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="17" t="s">
@@ -3604,13 +3619,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="76" thickBot="1">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -3618,25 +3633,25 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="17" t="s">
         <v>77</v>
       </c>
@@ -3676,10 +3691,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3692,12 +3707,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="20" t="s">
@@ -3741,118 +3756,130 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="10" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="10" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="10" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="10" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="21" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="10" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="21" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="10" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="10" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" thickBot="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="10" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="21" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="31" thickBot="1">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="21" t="s">
         <v>156</v>
       </c>
+    </row>
+    <row r="18" spans="1:4" ht="31" thickBot="1">
+      <c r="A18" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3891,12 +3918,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3940,12 +3967,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -4010,13 +4037,13 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="33" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -4024,17 +4051,17 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="7" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Add vote history detail
</commit_message>
<xml_diff>
--- a/Documents/Design/VoteInterfaceDocument.xlsx
+++ b/Documents/Design/VoteInterfaceDocument.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="25560" windowHeight="14080" tabRatio="624" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25560" windowHeight="14080" tabRatio="624" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="180">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -450,39 +450,195 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>state:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>participatorlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>participator's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emaillist:array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initiatorid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tokenid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>firstName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:signIn 1:signUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resendType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return when use Email signin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hasPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchtype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Response Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>optionlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>voteoptionid:int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>state:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>participatorlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>participator's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>emaillist:array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Request Content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>initiatorid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
+    <t>optionlist's subkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requestType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -494,11 +650,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tokenid</t>
+    <t>1:initiator 2:particitan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>currentvalidvote:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slectionlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servercurrentime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -506,19 +674,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lastName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
+    <t>oldpass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newpass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createtime:datetime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voteoptionid:int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -526,11 +718,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>firstName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isfinished</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -538,7 +730,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lastName</t>
+    <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -546,131 +738,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:signIn 1:signUp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>resendType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>return when use Email signin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hasPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchtype</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>double</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>latitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>longitude</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>array</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Response Content</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>optionlist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteoptionid:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>optionlist's subkey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>requestType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1:initiator 2:particitan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>currentvalidvote:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>createtime:datetime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>voteoptionid:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>slectionlist</t>
+    <t>endtime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -678,27 +750,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oldpass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>newpass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>content:string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -757,7 +809,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -882,43 +934,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -1033,7 +1048,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1101,7 +1116,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1138,15 +1156,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1594,40 +1603,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="39" customHeight="1" thickBot="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="5" t="s">
@@ -1642,10 +1651,10 @@
       <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="62" thickTop="1" thickBot="1">
       <c r="A6" s="6" t="s">
@@ -1660,10 +1669,10 @@
       <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="30"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="6" t="s">
@@ -1676,18 +1685,18 @@
         <v>11</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="16" thickTop="1">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1712,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1726,12 +1735,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="22" t="s">
@@ -1761,7 +1770,7 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>71</v>
@@ -1773,24 +1782,24 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>166</v>
       </c>
       <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1840,12 +1849,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1887,12 +1896,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -1942,12 +1951,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1977,12 +1986,12 @@
     </row>
     <row r="5" spans="1:5" ht="16" thickBot="1"/>
     <row r="6" spans="1:5" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:5" ht="16" thickBot="1">
       <c r="A7" s="18" t="s">
@@ -1999,13 +2008,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="31" thickBot="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -2013,19 +2022,19 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" thickBot="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="18" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" thickBot="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -2067,12 +2076,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2128,12 +2137,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="15" t="s">
@@ -2151,28 +2160,28 @@
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
       <c r="A9" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>135</v>
-      </c>
       <c r="C9" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:4" ht="31" thickBot="1">
       <c r="A10" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2193,10 +2202,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2210,12 +2219,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="10" t="s">
@@ -2245,75 +2254,75 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" thickBot="1">
       <c r="A8" s="36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>98</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="9" t="s">
-        <v>81</v>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="23" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="9" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="23" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="9" t="s">
-        <v>104</v>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="23" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
@@ -2326,25 +2335,85 @@
       <c r="C12" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="23" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="9" t="s">
-        <v>158</v>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="23" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" thickBot="1">
+      <c r="A15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="23"/>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1">
+      <c r="A16" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="16" thickBot="1">
+      <c r="A17" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" ht="31" thickBot="1">
+      <c r="A18" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="1:4" ht="16" thickBot="1">
+      <c r="A19" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2373,7 +2442,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2387,12 +2456,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2422,12 +2491,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="2" t="s">
@@ -2444,25 +2513,25 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="31" thickBot="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="2" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2503,12 +2572,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="12" t="s">
@@ -2526,7 +2595,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>42</v>
@@ -2538,24 +2607,24 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="12" t="s">
@@ -2568,7 +2637,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2606,12 +2675,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="16" t="s">
@@ -2632,7 +2701,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>12</v>
@@ -2641,50 +2710,50 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>129</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="14" t="s">
@@ -2735,12 +2804,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="14" t="s">
@@ -2758,7 +2827,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>42</v>
@@ -2770,12 +2839,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="14" t="s">
@@ -2843,12 +2912,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="A1" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -2866,7 +2935,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -2890,7 +2959,7 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -2902,12 +2971,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -2958,12 +3027,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="19" t="s">
@@ -2981,7 +3050,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>42</v>
@@ -2993,12 +3062,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="19" t="s">
@@ -3047,12 +3116,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3082,12 +3151,12 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1"/>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="13" t="s">
@@ -3136,12 +3205,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3183,12 +3252,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="15" t="s">
@@ -3206,13 +3275,13 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>133</v>
-      </c>
       <c r="C8" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -3249,12 +3318,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3382,12 +3451,12 @@
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1"/>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="7" t="s">
@@ -3449,12 +3518,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3496,12 +3565,12 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" thickBot="1">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="7" t="s">
@@ -3551,12 +3620,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3588,10 +3657,10 @@
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>36</v>
@@ -3600,10 +3669,10 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -3624,12 +3693,12 @@
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1"/>
     <row r="9" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="17" t="s">
@@ -3646,13 +3715,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="76" thickBot="1">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="36" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -3660,38 +3729,38 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
       <c r="A15" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="C15" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>141</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>67</v>
@@ -3721,7 +3790,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3734,12 +3803,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="20" t="s">
@@ -3769,26 +3838,26 @@
     </row>
     <row r="4" spans="1:4" ht="31" thickBot="1">
       <c r="A4" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1"/>
     <row r="6" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1">
       <c r="A7" s="21" t="s">
@@ -3805,13 +3874,13 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>79</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -3819,92 +3888,92 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31" thickBot="1">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="21" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" thickBot="1">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="31" thickBot="1">
       <c r="A17" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="C17" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="D17" s="21" t="s">
         <v>154</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="31" thickBot="1">
       <c r="A18" s="21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D18" s="21"/>
     </row>
@@ -3932,7 +4001,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3945,12 +4014,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -3994,12 +4063,12 @@
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1"/>
     <row r="7" spans="1:4" ht="16" customHeight="1" thickBot="1">
-      <c r="A7" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="A7" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="7" t="s">
@@ -4032,7 +4101,7 @@
         <v>73</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>75</v>
@@ -4044,7 +4113,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>18</v>
@@ -4064,33 +4133,33 @@
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" ht="31" thickBot="1">
-      <c r="A13" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="34" t="s">
+      <c r="A13" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="35" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>